<commit_message>
Updated cheatsheet for MFC data
</commit_message>
<xml_diff>
--- a/MFC_Tests/MFC_Tests_Cheatsheet.xlsx
+++ b/MFC_Tests/MFC_Tests_Cheatsheet.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="116">
   <si>
     <t>EntryNumber</t>
   </si>
@@ -340,6 +340,24 @@
   </si>
   <si>
     <t>10/24/2022 - Board2 - NO, RH, O2</t>
+  </si>
+  <si>
+    <t>10/25/2022 - Board0 - NO, RH, O2</t>
+  </si>
+  <si>
+    <t>10/25/2022 - Board1 - NO, RH, O2</t>
+  </si>
+  <si>
+    <t>10/25/2022 - Board2 - NO, RH, O2</t>
+  </si>
+  <si>
+    <t>10/26/2022 - Board0 - NO, RH, O2</t>
+  </si>
+  <si>
+    <t>10/26/2022 - Board1 - NO, RH, O2</t>
+  </si>
+  <si>
+    <t>10/26/2022 - Board2 - NO, RH, O2</t>
   </si>
   <si>
     <t>ExtraComments</t>
@@ -388,7 +406,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E94"/>
+  <dimension ref="A1:E100"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="true"/>
@@ -412,7 +430,7 @@
         <v>15</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2">
@@ -1810,6 +1828,96 @@
       </c>
       <c r="E94" s="0"/>
     </row>
+    <row r="95">
+      <c r="A95" s="0">
+        <v>95</v>
+      </c>
+      <c r="B95" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C95" s="0">
+        <v>18</v>
+      </c>
+      <c r="D95" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="E95" s="0"/>
+    </row>
+    <row r="96">
+      <c r="A96" s="0">
+        <v>96</v>
+      </c>
+      <c r="B96" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C96" s="0">
+        <v>19</v>
+      </c>
+      <c r="D96" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="E96" s="0"/>
+    </row>
+    <row r="97">
+      <c r="A97" s="0">
+        <v>97</v>
+      </c>
+      <c r="B97" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C97" s="0">
+        <v>17</v>
+      </c>
+      <c r="D97" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="E97" s="0"/>
+    </row>
+    <row r="98">
+      <c r="A98" s="0">
+        <v>98</v>
+      </c>
+      <c r="B98" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C98" s="0">
+        <v>18</v>
+      </c>
+      <c r="D98" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="E98" s="0"/>
+    </row>
+    <row r="99">
+      <c r="A99" s="0">
+        <v>99</v>
+      </c>
+      <c r="B99" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C99" s="0">
+        <v>19</v>
+      </c>
+      <c r="D99" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="E99" s="0"/>
+    </row>
+    <row r="100">
+      <c r="A100" s="0">
+        <v>100</v>
+      </c>
+      <c r="B100" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="C100" s="0">
+        <v>17</v>
+      </c>
+      <c r="D100" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="E100" s="0"/>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>